<commit_message>
Added Corruption perceptions index to Africa dataset
Added Corruption perceptions index to Africa dataset
</commit_message>
<xml_diff>
--- a/Africa.xlsx
+++ b/Africa.xlsx
@@ -37,175 +37,175 @@
     <t>FCO Travel Advice</t>
   </si>
   <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Not Free</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Bostwana</t>
+  </si>
+  <si>
+    <t>Burkino Faso</t>
+  </si>
+  <si>
+    <t>Partly Free</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Cape verde</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Ethopia</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guinea Bissau</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the congo</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>São Tomé and Príncipe</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Somaila</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Tazania</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
     <t>Zimbabwe</t>
-  </si>
-  <si>
-    <t>Not Free</t>
-  </si>
-  <si>
-    <t>Zambia</t>
-  </si>
-  <si>
-    <t>Partly Free</t>
-  </si>
-  <si>
-    <t>Uganda</t>
-  </si>
-  <si>
-    <t>Tunisia</t>
-  </si>
-  <si>
-    <t>Togo</t>
-  </si>
-  <si>
-    <t>Tazania</t>
-  </si>
-  <si>
-    <t>Swaziland</t>
-  </si>
-  <si>
-    <t>Sudan</t>
-  </si>
-  <si>
-    <t>South Sudan</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Free</t>
-  </si>
-  <si>
-    <t>Somaila</t>
-  </si>
-  <si>
-    <t>Sierra Leone</t>
-  </si>
-  <si>
-    <t>Seychelles</t>
-  </si>
-  <si>
-    <t>Senegal</t>
-  </si>
-  <si>
-    <t>São Tomé and Príncipe</t>
-  </si>
-  <si>
-    <t>Rwanda</t>
-  </si>
-  <si>
-    <t>Republic of the congo</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>Niger</t>
-  </si>
-  <si>
-    <t>Namibia</t>
-  </si>
-  <si>
-    <t>Mozambique</t>
-  </si>
-  <si>
-    <t>Morocco</t>
-  </si>
-  <si>
-    <t>Mauritius</t>
-  </si>
-  <si>
-    <t>Mauritania</t>
-  </si>
-  <si>
-    <t>Mali</t>
-  </si>
-  <si>
-    <t>Malawi</t>
-  </si>
-  <si>
-    <t>Madagascar</t>
-  </si>
-  <si>
-    <t>Libya</t>
-  </si>
-  <si>
-    <t>Liberia</t>
-  </si>
-  <si>
-    <t>Lesotho</t>
-  </si>
-  <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>Guinea Bissau</t>
-  </si>
-  <si>
-    <t>Guiea</t>
-  </si>
-  <si>
-    <t>Ghana</t>
-  </si>
-  <si>
-    <t>Gambia</t>
-  </si>
-  <si>
-    <t>Gabon</t>
-  </si>
-  <si>
-    <t>Ethopia</t>
-  </si>
-  <si>
-    <t>Eritrea</t>
-  </si>
-  <si>
-    <t>Equatorial Guinea</t>
-  </si>
-  <si>
-    <t>Egypt</t>
-  </si>
-  <si>
-    <t>Djibouti</t>
-  </si>
-  <si>
-    <t>Democratic Republic of the Congo</t>
-  </si>
-  <si>
-    <t>Côte d'Ivoire</t>
-  </si>
-  <si>
-    <t>Comoros</t>
-  </si>
-  <si>
-    <t>Chad</t>
-  </si>
-  <si>
-    <t>Central African Republic</t>
-  </si>
-  <si>
-    <t>Cape verde</t>
-  </si>
-  <si>
-    <t>Cameroon</t>
-  </si>
-  <si>
-    <t>Burundi</t>
-  </si>
-  <si>
-    <t>Burkino Faso</t>
-  </si>
-  <si>
-    <t>Bostwana</t>
-  </si>
-  <si>
-    <t>Benin</t>
-  </si>
-  <si>
-    <t>Angola</t>
-  </si>
-  <si>
-    <t>Algeria</t>
   </si>
 </sst>
 </file>
@@ -364,10 +364,13 @@
         <v>8</v>
       </c>
       <c s="2" r="C2">
-        <v>2607</v>
+        <v>7124</v>
       </c>
       <c r="D2">
-        <v>13010000</v>
+        <v>33333216</v>
+      </c>
+      <c r="E2">
+        <v>34</v>
       </c>
       <c t="s" r="F2">
         <v>9</v>
@@ -378,27 +381,33 @@
         <v>10</v>
       </c>
       <c s="2" r="C3">
-        <v>931</v>
+        <v>2813</v>
       </c>
       <c r="D3">
-        <v>14668000</v>
+        <v>15941000</v>
+      </c>
+      <c r="E3">
+        <v>22</v>
       </c>
       <c t="s" r="F3">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="3" r="A4">
+        <v>11</v>
+      </c>
+      <c s="2" r="C4">
+        <v>1176</v>
+      </c>
+      <c r="D4">
+        <v>8439000</v>
+      </c>
+      <c r="E4">
+        <v>36</v>
+      </c>
+      <c t="s" r="F4">
         <v>12</v>
-      </c>
-      <c s="2" r="C4">
-        <v>1700</v>
-      </c>
-      <c r="D4">
-        <v>27616000</v>
-      </c>
-      <c t="s" r="F4">
-        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -406,13 +415,16 @@
         <v>13</v>
       </c>
       <c s="2" r="C5">
-        <v>8800</v>
+        <v>11400</v>
       </c>
       <c r="D5">
-        <v>10102000</v>
+        <v>1839833</v>
+      </c>
+      <c r="E5">
+        <v>65</v>
       </c>
       <c t="s" r="F5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -420,38 +432,47 @@
         <v>14</v>
       </c>
       <c s="2" r="C6">
-        <v>1700</v>
+        <v>1284</v>
       </c>
       <c r="D6">
-        <v>6100000</v>
+        <v>13228000</v>
+      </c>
+      <c r="E6">
+        <v>38</v>
       </c>
       <c t="s" r="F6">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="3" r="A7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c s="2" r="C7">
-        <v>723</v>
+        <v>739</v>
       </c>
       <c r="D7">
-        <v>44929002</v>
+        <v>7548000</v>
+      </c>
+      <c r="E7">
+        <v>19</v>
       </c>
       <c t="s" r="F7">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="3" r="A8">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c s="2" r="C8">
-        <v>5245</v>
+        <v>2421</v>
       </c>
       <c r="D8">
-        <v>1032000</v>
+        <v>17795000</v>
+      </c>
+      <c r="E8">
+        <v>26</v>
       </c>
       <c t="s" r="F8">
         <v>9</v>
@@ -459,44 +480,53 @@
     </row>
     <row r="9">
       <c t="s" s="3" r="A9">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c s="2" r="C9">
-        <v>2300</v>
+        <v>6418</v>
       </c>
       <c r="D9">
-        <v>36787012</v>
+        <v>420979</v>
+      </c>
+      <c r="E9">
+        <v>60</v>
       </c>
       <c t="s" r="F9">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="3" r="A10">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c s="2" r="C10">
-        <v>1546</v>
+        <v>1198</v>
       </c>
       <c r="D10">
-        <v>8260490</v>
+        <v>4216666</v>
+      </c>
+      <c r="E10">
+        <v>26</v>
       </c>
       <c t="s" r="F10">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="3" r="A11">
+        <v>20</v>
+      </c>
+      <c s="2" r="C11">
+        <v>1519</v>
+      </c>
+      <c r="D11">
+        <v>10146000</v>
+      </c>
+      <c r="E11">
         <v>19</v>
       </c>
-      <c s="2" r="C11">
-        <v>12161</v>
-      </c>
-      <c r="D11">
-        <v>47432000</v>
-      </c>
       <c t="s" r="F11">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -504,13 +534,16 @@
         <v>21</v>
       </c>
       <c s="2" r="C12">
-        <v>600</v>
+        <v>1660</v>
       </c>
       <c r="D12">
-        <v>9832017</v>
+        <v>798000</v>
+      </c>
+      <c r="E12">
+        <v>28</v>
       </c>
       <c t="s" r="F12">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -518,13 +551,16 @@
         <v>22</v>
       </c>
       <c s="2" r="C13">
-        <v>903</v>
+        <v>1600</v>
       </c>
       <c r="D13">
-        <v>6144562</v>
+        <v>17654843</v>
+      </c>
+      <c r="E13">
+        <v>29</v>
       </c>
       <c t="s" r="F13">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
@@ -532,13 +568,16 @@
         <v>23</v>
       </c>
       <c s="2" r="C14">
-        <v>11818</v>
+        <v>774</v>
       </c>
       <c r="D14">
-        <v>80654</v>
+        <v>71712867</v>
+      </c>
+      <c r="E14">
+        <v>21</v>
       </c>
       <c t="s" r="F14">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -546,13 +585,16 @@
         <v>24</v>
       </c>
       <c s="2" r="C15">
-        <v>1759</v>
+        <v>2070</v>
       </c>
       <c r="D15">
-        <v>11658000</v>
+        <v>906000</v>
+      </c>
+      <c r="E15">
+        <v>36</v>
       </c>
       <c t="s" r="F15">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
@@ -560,13 +602,16 @@
         <v>25</v>
       </c>
       <c s="2" r="C16">
-        <v>1226</v>
+        <v>4836</v>
       </c>
       <c r="D16">
-        <v>157000</v>
+        <v>80335036</v>
+      </c>
+      <c r="E16">
+        <v>32</v>
       </c>
       <c t="s" r="F16">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
@@ -574,10 +619,13 @@
         <v>26</v>
       </c>
       <c s="2" r="C17">
-        <v>1300</v>
+        <v>16312</v>
       </c>
       <c r="D17">
-        <v>7600000</v>
+        <v>504000</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
       </c>
       <c t="s" r="F17">
         <v>9</v>
@@ -588,10 +636,13 @@
         <v>27</v>
       </c>
       <c s="2" r="C18">
-        <v>3919</v>
+        <v>1000</v>
       </c>
       <c r="D18">
-        <v>4012809</v>
+        <v>5880000</v>
+      </c>
+      <c r="E18">
+        <v>25</v>
       </c>
       <c t="s" r="F18">
         <v>9</v>
@@ -602,13 +653,16 @@
         <v>28</v>
       </c>
       <c s="2" r="C19">
-        <v>1188</v>
+        <v>1100</v>
       </c>
       <c r="D19">
-        <v>154729000</v>
+        <v>85237338</v>
+      </c>
+      <c r="E19">
+        <v>33</v>
       </c>
       <c t="s" r="F19">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
@@ -616,13 +670,16 @@
         <v>29</v>
       </c>
       <c s="2" r="C20">
-        <v>872</v>
+        <v>7055</v>
       </c>
       <c r="D20">
-        <v>13957000</v>
+        <v>1384000</v>
+      </c>
+      <c r="E20">
+        <v>35</v>
       </c>
       <c t="s" r="F20">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -630,13 +687,16 @@
         <v>30</v>
       </c>
       <c s="2" r="C21">
-        <v>7478</v>
+        <v>2002</v>
       </c>
       <c r="D21">
-        <v>2031000</v>
+        <v>1517000</v>
+      </c>
+      <c r="E21">
+        <v>34</v>
       </c>
       <c t="s" r="F21">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22">
@@ -644,13 +704,16 @@
         <v>31</v>
       </c>
       <c s="2" r="C22">
-        <v>1389</v>
+        <v>2700</v>
       </c>
       <c r="D22">
-        <v>20366795</v>
+        <v>23000000</v>
+      </c>
+      <c r="E22">
+        <v>45</v>
       </c>
       <c t="s" r="F22">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
@@ -658,13 +721,16 @@
         <v>32</v>
       </c>
       <c s="2" r="C23">
-        <v>4600</v>
+        <v>2035</v>
       </c>
       <c r="D23">
-        <v>35757175</v>
+        <v>9402000</v>
+      </c>
+      <c r="E23">
+        <v>24</v>
       </c>
       <c t="s" r="F23">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
@@ -672,13 +738,16 @@
         <v>33</v>
       </c>
       <c s="2" r="C24">
-        <v>13703</v>
+        <v>736</v>
       </c>
       <c r="D24">
-        <v>1219220</v>
+        <v>1586000</v>
+      </c>
+      <c r="E24">
+        <v>25</v>
       </c>
       <c t="s" r="F24">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
@@ -686,13 +755,16 @@
         <v>34</v>
       </c>
       <c s="2" r="C25">
-        <v>2402</v>
+        <v>1445</v>
       </c>
       <c r="D25">
-        <v>3069000</v>
+        <v>34707817</v>
+      </c>
+      <c r="E25">
+        <v>27</v>
       </c>
       <c t="s" r="F25">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26">
@@ -700,13 +772,16 @@
         <v>35</v>
       </c>
       <c s="2" r="C26">
-        <v>1154</v>
+        <v>2113</v>
       </c>
       <c r="D26">
-        <v>13518000</v>
+        <v>1795000</v>
+      </c>
+      <c r="E26">
+        <v>45</v>
       </c>
       <c t="s" r="F26">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
@@ -714,13 +789,16 @@
         <v>36</v>
       </c>
       <c s="2" r="C27">
-        <v>596</v>
+        <v>1003</v>
       </c>
       <c r="D27">
-        <v>12884000</v>
+        <v>3283000</v>
+      </c>
+      <c r="E27">
+        <v>41</v>
       </c>
       <c t="s" r="F27">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
@@ -728,13 +806,16 @@
         <v>37</v>
       </c>
       <c s="2" r="C28">
-        <v>905</v>
+        <v>12700</v>
       </c>
       <c r="D28">
-        <v>18606000</v>
+        <v>6036914</v>
+      </c>
+      <c r="E28">
+        <v>21</v>
       </c>
       <c t="s" r="F28">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
@@ -742,13 +823,16 @@
         <v>38</v>
       </c>
       <c s="2" r="C29">
-        <v>12700</v>
+        <v>905</v>
       </c>
       <c r="D29">
-        <v>6036914</v>
+        <v>18606000</v>
+      </c>
+      <c r="E29">
+        <v>32</v>
       </c>
       <c t="s" r="F29">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30">
@@ -756,13 +840,16 @@
         <v>39</v>
       </c>
       <c s="2" r="C30">
-        <v>1003</v>
+        <v>596</v>
       </c>
       <c r="D30">
-        <v>3283000</v>
+        <v>12884000</v>
+      </c>
+      <c r="E30">
+        <v>37</v>
       </c>
       <c t="s" r="F30">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31">
@@ -770,13 +857,16 @@
         <v>40</v>
       </c>
       <c s="2" r="C31">
-        <v>2113</v>
+        <v>1154</v>
       </c>
       <c r="D31">
-        <v>1795000</v>
+        <v>13518000</v>
+      </c>
+      <c r="E31">
+        <v>37</v>
       </c>
       <c t="s" r="F31">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
@@ -784,13 +874,16 @@
         <v>41</v>
       </c>
       <c s="2" r="C32">
-        <v>1445</v>
+        <v>2402</v>
       </c>
       <c r="D32">
-        <v>34707817</v>
+        <v>3069000</v>
+      </c>
+      <c r="E32">
+        <v>31</v>
       </c>
       <c t="s" r="F32">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33">
@@ -798,13 +891,16 @@
         <v>42</v>
       </c>
       <c s="2" r="C33">
-        <v>736</v>
+        <v>13703</v>
       </c>
       <c r="D33">
-        <v>1586000</v>
+        <v>1219220</v>
+      </c>
+      <c r="E33">
+        <v>57</v>
       </c>
       <c t="s" r="F33">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34">
@@ -812,13 +908,16 @@
         <v>43</v>
       </c>
       <c s="2" r="C34">
-        <v>2035</v>
+        <v>4600</v>
       </c>
       <c r="D34">
-        <v>9402000</v>
+        <v>35757175</v>
+      </c>
+      <c r="E34">
+        <v>37</v>
       </c>
       <c t="s" r="F34">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35">
@@ -826,13 +925,16 @@
         <v>44</v>
       </c>
       <c s="2" r="C35">
-        <v>2700</v>
+        <v>1389</v>
       </c>
       <c r="D35">
-        <v>23000000</v>
+        <v>20366795</v>
+      </c>
+      <c r="E35">
+        <v>31</v>
       </c>
       <c t="s" r="F35">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36">
@@ -840,13 +942,16 @@
         <v>45</v>
       </c>
       <c s="2" r="C36">
-        <v>2002</v>
+        <v>7478</v>
       </c>
       <c r="D36">
-        <v>1517000</v>
+        <v>2031000</v>
+      </c>
+      <c r="E36">
+        <v>48</v>
       </c>
       <c t="s" r="F36">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
@@ -854,13 +959,16 @@
         <v>46</v>
       </c>
       <c s="2" r="C37">
-        <v>7055</v>
+        <v>872</v>
       </c>
       <c r="D37">
-        <v>1384000</v>
+        <v>13957000</v>
+      </c>
+      <c r="E37">
+        <v>48</v>
       </c>
       <c t="s" r="F37">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38">
@@ -868,13 +976,16 @@
         <v>47</v>
       </c>
       <c s="2" r="C38">
-        <v>1100</v>
+        <v>1188</v>
       </c>
       <c r="D38">
-        <v>85237338</v>
+        <v>154729000</v>
+      </c>
+      <c r="E38">
+        <v>33</v>
       </c>
       <c t="s" r="F38">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39">
@@ -882,10 +993,13 @@
         <v>48</v>
       </c>
       <c s="2" r="C39">
-        <v>1000</v>
+        <v>3919</v>
       </c>
       <c r="D39">
-        <v>5880000</v>
+        <v>4012809</v>
+      </c>
+      <c r="E39">
+        <v>21</v>
       </c>
       <c t="s" r="F39">
         <v>9</v>
@@ -896,10 +1010,13 @@
         <v>49</v>
       </c>
       <c s="2" r="C40">
-        <v>16312</v>
+        <v>1300</v>
       </c>
       <c r="D40">
-        <v>504000</v>
+        <v>7600000</v>
+      </c>
+      <c r="E40">
+        <v>53</v>
       </c>
       <c t="s" r="F40">
         <v>9</v>
@@ -910,13 +1027,16 @@
         <v>50</v>
       </c>
       <c s="2" r="C41">
-        <v>4836</v>
+        <v>1226</v>
       </c>
       <c r="D41">
-        <v>80335036</v>
+        <v>157000</v>
+      </c>
+      <c r="E41">
+        <v>42</v>
       </c>
       <c t="s" r="F41">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42">
@@ -924,13 +1044,16 @@
         <v>51</v>
       </c>
       <c s="2" r="C42">
-        <v>2070</v>
+        <v>1759</v>
       </c>
       <c r="D42">
-        <v>906000</v>
+        <v>11658000</v>
+      </c>
+      <c r="E42">
+        <v>36</v>
       </c>
       <c t="s" r="F42">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43">
@@ -938,13 +1061,16 @@
         <v>52</v>
       </c>
       <c s="2" r="C43">
-        <v>774</v>
+        <v>11818</v>
       </c>
       <c r="D43">
-        <v>71712867</v>
+        <v>80654</v>
+      </c>
+      <c r="E43">
+        <v>52</v>
       </c>
       <c t="s" r="F43">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44">
@@ -952,13 +1078,16 @@
         <v>53</v>
       </c>
       <c s="2" r="C44">
-        <v>1600</v>
+        <v>903</v>
       </c>
       <c r="D44">
-        <v>17654843</v>
+        <v>6144562</v>
+      </c>
+      <c r="E44">
+        <v>31</v>
       </c>
       <c t="s" r="F44">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45">
@@ -966,13 +1095,16 @@
         <v>54</v>
       </c>
       <c s="2" r="C45">
-        <v>1660</v>
+        <v>600</v>
       </c>
       <c r="D45">
-        <v>798000</v>
+        <v>9832017</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
       </c>
       <c t="s" r="F45">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46">
@@ -980,13 +1112,16 @@
         <v>55</v>
       </c>
       <c s="2" r="C46">
-        <v>1519</v>
+        <v>12161</v>
       </c>
       <c r="D46">
-        <v>10146000</v>
+        <v>47432000</v>
+      </c>
+      <c r="E46">
+        <v>43</v>
       </c>
       <c t="s" r="F46">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47">
@@ -994,13 +1129,13 @@
         <v>56</v>
       </c>
       <c s="2" r="C47">
-        <v>1198</v>
+        <v>1546</v>
       </c>
       <c r="D47">
-        <v>4216666</v>
+        <v>8260490</v>
       </c>
       <c t="s" r="F47">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
@@ -1008,13 +1143,16 @@
         <v>57</v>
       </c>
       <c s="2" r="C48">
-        <v>6418</v>
+        <v>2300</v>
       </c>
       <c r="D48">
-        <v>420979</v>
+        <v>36787012</v>
+      </c>
+      <c r="E48">
+        <v>13</v>
       </c>
       <c t="s" r="F48">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
@@ -1022,10 +1160,13 @@
         <v>58</v>
       </c>
       <c s="2" r="C49">
-        <v>2421</v>
+        <v>5245</v>
       </c>
       <c r="D49">
-        <v>17795000</v>
+        <v>1032000</v>
+      </c>
+      <c r="E49">
+        <v>37</v>
       </c>
       <c t="s" r="F49">
         <v>9</v>
@@ -1036,13 +1177,16 @@
         <v>59</v>
       </c>
       <c s="2" r="C50">
-        <v>739</v>
+        <v>723</v>
       </c>
       <c r="D50">
-        <v>7548000</v>
+        <v>44929002</v>
+      </c>
+      <c r="E50">
+        <v>35</v>
       </c>
       <c t="s" r="F50">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51">
@@ -1050,13 +1194,16 @@
         <v>60</v>
       </c>
       <c s="2" r="C51">
-        <v>1284</v>
+        <v>1700</v>
       </c>
       <c r="D51">
-        <v>13228000</v>
+        <v>6100000</v>
+      </c>
+      <c r="E51">
+        <v>30</v>
       </c>
       <c t="s" r="F51">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52">
@@ -1064,13 +1211,16 @@
         <v>61</v>
       </c>
       <c s="2" r="C52">
-        <v>11400</v>
+        <v>8800</v>
       </c>
       <c r="D52">
-        <v>1839833</v>
+        <v>10102000</v>
+      </c>
+      <c r="E52">
+        <v>41</v>
       </c>
       <c t="s" r="F52">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53">
@@ -1078,13 +1228,16 @@
         <v>62</v>
       </c>
       <c s="2" r="C53">
-        <v>1176</v>
+        <v>1700</v>
       </c>
       <c r="D53">
-        <v>8439000</v>
+        <v>27616000</v>
+      </c>
+      <c r="E53">
+        <v>29</v>
       </c>
       <c t="s" r="F53">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54">
@@ -1092,13 +1245,16 @@
         <v>63</v>
       </c>
       <c s="2" r="C54">
-        <v>2813</v>
+        <v>931</v>
       </c>
       <c r="D54">
-        <v>15941000</v>
+        <v>14668000</v>
+      </c>
+      <c r="E54">
+        <v>37</v>
       </c>
       <c t="s" r="F54">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55">
@@ -1106,10 +1262,13 @@
         <v>64</v>
       </c>
       <c s="2" r="C55">
-        <v>7124</v>
+        <v>2607</v>
       </c>
       <c r="D55">
-        <v>33333216</v>
+        <v>13010000</v>
+      </c>
+      <c r="E55">
+        <v>20</v>
       </c>
       <c t="s" r="F55">
         <v>9</v>

</xml_diff>

<commit_message>
Adds FCO Travel Advice
Adds FCO travel advice to the Afria Database for candidate filtering
</commit_message>
<xml_diff>
--- a/Africa.xlsx
+++ b/Africa.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
   <si>
     <t>Country</t>
   </si>
@@ -31,10 +31,7 @@
     <t>Freedom index</t>
   </si>
   <si>
-    <t>African Union</t>
-  </si>
-  <si>
-    <t>FCO Travel Advice</t>
+    <t>FCO Travel Advice (Jan 2013)</t>
   </si>
   <si>
     <t>Algeria</t>
@@ -43,6 +40,9 @@
     <t>Not Free</t>
   </si>
   <si>
+    <t>Avoid all but essential travel to part(s) of country</t>
+  </si>
+  <si>
     <t>Angola</t>
   </si>
   <si>
@@ -52,6 +52,9 @@
     <t>Free</t>
   </si>
   <si>
+    <t>No restrictions in this travel advice</t>
+  </si>
+  <si>
     <t>Bostwana</t>
   </si>
   <si>
@@ -61,9 +64,15 @@
     <t>Partly Free</t>
   </si>
   <si>
+    <t>Avoid all travel to part(s) of country</t>
+  </si>
+  <si>
     <t>Burundi</t>
   </si>
   <si>
+    <t>Avoid all travel to whole country</t>
+  </si>
+  <si>
     <t>Cameroon</t>
   </si>
   <si>
@@ -161,6 +170,9 @@
   </si>
   <si>
     <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Avoid all but essential travel to whole country</t>
   </si>
   <si>
     <t>São Tomé and Príncipe</t>
@@ -284,10 +296,20 @@
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FFFF9900"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF93C47D"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -319,6 +341,7 @@
     <col min="3" customWidth="1" max="3" width="15.57"/>
     <col min="4" customWidth="1" max="4" width="11.14"/>
     <col min="6" customWidth="1" max="6" width="15.57"/>
+    <col min="7" customWidth="1" max="7" width="44.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -343,9 +366,7 @@
       <c t="s" s="3" r="G1">
         <v>6</v>
       </c>
-      <c t="s" s="3" r="H1">
-        <v>7</v>
-      </c>
+      <c s="3" r="H1"/>
       <c s="3" r="I1"/>
       <c s="3" r="J1"/>
       <c s="3" r="K1"/>
@@ -361,7 +382,7 @@
     </row>
     <row r="2">
       <c t="s" s="3" r="A2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c s="2" r="C2">
         <v>7124</v>
@@ -373,6 +394,9 @@
         <v>34</v>
       </c>
       <c t="s" r="F2">
+        <v>8</v>
+      </c>
+      <c t="s" r="G2">
         <v>9</v>
       </c>
     </row>
@@ -390,6 +414,9 @@
         <v>22</v>
       </c>
       <c t="s" r="F3">
+        <v>8</v>
+      </c>
+      <c t="s" r="G3">
         <v>9</v>
       </c>
     </row>
@@ -409,10 +436,13 @@
       <c t="s" r="F4">
         <v>12</v>
       </c>
+      <c t="s" r="G4">
+        <v>13</v>
+      </c>
     </row>
     <row r="5">
       <c t="s" s="3" r="A5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c s="2" r="C5">
         <v>11400</v>
@@ -426,10 +456,13 @@
       <c t="s" r="F5">
         <v>12</v>
       </c>
+      <c t="s" r="G5">
+        <v>13</v>
+      </c>
     </row>
     <row r="6">
       <c t="s" s="3" r="A6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c s="2" r="C6">
         <v>1284</v>
@@ -441,12 +474,15 @@
         <v>38</v>
       </c>
       <c t="s" r="F6">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G6">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="3" r="A7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c s="2" r="C7">
         <v>739</v>
@@ -458,12 +494,15 @@
         <v>19</v>
       </c>
       <c t="s" r="F7">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G7">
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="3" r="A8">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c s="2" r="C8">
         <v>2421</v>
@@ -475,12 +514,15 @@
         <v>26</v>
       </c>
       <c t="s" r="F8">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G8">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="3" r="A9">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c s="2" r="C9">
         <v>6418</v>
@@ -494,10 +536,13 @@
       <c t="s" r="F9">
         <v>12</v>
       </c>
+      <c t="s" r="G9">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c t="s" s="3" r="A10">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c s="2" r="C10">
         <v>1198</v>
@@ -509,12 +554,15 @@
         <v>26</v>
       </c>
       <c t="s" r="F10">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G10">
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="3" r="A11">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c s="2" r="C11">
         <v>1519</v>
@@ -526,12 +574,15 @@
         <v>19</v>
       </c>
       <c t="s" r="F11">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G11">
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="3" r="A12">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c s="2" r="C12">
         <v>1660</v>
@@ -543,12 +594,15 @@
         <v>28</v>
       </c>
       <c t="s" r="F12">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G12">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="3" r="A13">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c s="2" r="C13">
         <v>1600</v>
@@ -560,12 +614,15 @@
         <v>29</v>
       </c>
       <c t="s" r="F13">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G13">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="3" r="A14">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c s="2" r="C14">
         <v>774</v>
@@ -577,12 +634,15 @@
         <v>21</v>
       </c>
       <c t="s" r="F14">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G14">
+        <v>19</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="3" r="A15">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c s="2" r="C15">
         <v>2070</v>
@@ -594,12 +654,15 @@
         <v>36</v>
       </c>
       <c t="s" r="F15">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G15">
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="3" r="A16">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c s="2" r="C16">
         <v>4836</v>
@@ -611,12 +674,15 @@
         <v>32</v>
       </c>
       <c t="s" r="F16">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G16">
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="3" r="A17">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c s="2" r="C17">
         <v>16312</v>
@@ -628,12 +694,15 @@
         <v>20</v>
       </c>
       <c t="s" r="F17">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G17">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="3" r="A18">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c s="2" r="C18">
         <v>1000</v>
@@ -645,12 +714,15 @@
         <v>25</v>
       </c>
       <c t="s" r="F18">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G18">
+        <v>17</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="3" r="A19">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c s="2" r="C19">
         <v>1100</v>
@@ -662,12 +734,15 @@
         <v>33</v>
       </c>
       <c t="s" r="F19">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G19">
+        <v>17</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="3" r="A20">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c s="2" r="C20">
         <v>7055</v>
@@ -679,12 +754,15 @@
         <v>35</v>
       </c>
       <c t="s" r="F20">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G20">
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="3" r="A21">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c s="2" r="C21">
         <v>2002</v>
@@ -696,12 +774,15 @@
         <v>34</v>
       </c>
       <c t="s" r="F21">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G21">
+        <v>13</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="3" r="A22">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c s="2" r="C22">
         <v>2700</v>
@@ -715,10 +796,13 @@
       <c t="s" r="F22">
         <v>12</v>
       </c>
+      <c t="s" r="G22">
+        <v>13</v>
+      </c>
     </row>
     <row r="23">
       <c t="s" s="3" r="A23">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c s="2" r="C23">
         <v>2035</v>
@@ -730,12 +814,15 @@
         <v>24</v>
       </c>
       <c t="s" r="F23">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G23">
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c t="s" s="3" r="A24">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c s="2" r="C24">
         <v>736</v>
@@ -747,12 +834,15 @@
         <v>25</v>
       </c>
       <c t="s" r="F24">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G24">
+        <v>13</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="3" r="A25">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c s="2" r="C25">
         <v>1445</v>
@@ -764,12 +854,15 @@
         <v>27</v>
       </c>
       <c t="s" r="F25">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G25">
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="3" r="A26">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c s="2" r="C26">
         <v>2113</v>
@@ -783,10 +876,13 @@
       <c t="s" r="F26">
         <v>12</v>
       </c>
+      <c t="s" r="G26">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c t="s" s="3" r="A27">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c s="2" r="C27">
         <v>1003</v>
@@ -798,12 +894,15 @@
         <v>41</v>
       </c>
       <c t="s" r="F27">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G27">
+        <v>9</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="3" r="A28">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c s="2" r="C28">
         <v>12700</v>
@@ -815,12 +914,15 @@
         <v>21</v>
       </c>
       <c t="s" r="F28">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G28">
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="3" r="A29">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c s="2" r="C29">
         <v>905</v>
@@ -832,12 +934,15 @@
         <v>32</v>
       </c>
       <c t="s" r="F29">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G29">
+        <v>19</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="3" r="A30">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c s="2" r="C30">
         <v>596</v>
@@ -849,12 +954,15 @@
         <v>37</v>
       </c>
       <c t="s" r="F30">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G30">
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="3" r="A31">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c s="2" r="C31">
         <v>1154</v>
@@ -866,12 +974,15 @@
         <v>37</v>
       </c>
       <c t="s" r="F31">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G31">
+        <v>19</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="3" r="A32">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c s="2" r="C32">
         <v>2402</v>
@@ -883,12 +994,15 @@
         <v>31</v>
       </c>
       <c t="s" r="F32">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G32">
+        <v>19</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="3" r="A33">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c s="2" r="C33">
         <v>13703</v>
@@ -902,10 +1016,13 @@
       <c t="s" r="F33">
         <v>12</v>
       </c>
+      <c t="s" r="G33">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c t="s" s="3" r="A34">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c s="2" r="C34">
         <v>4600</v>
@@ -917,12 +1034,15 @@
         <v>37</v>
       </c>
       <c t="s" r="F34">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G34">
+        <v>13</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="3" r="A35">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c s="2" r="C35">
         <v>1389</v>
@@ -934,12 +1054,15 @@
         <v>31</v>
       </c>
       <c t="s" r="F35">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G35">
+        <v>13</v>
       </c>
     </row>
     <row r="36">
       <c t="s" s="3" r="A36">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c s="2" r="C36">
         <v>7478</v>
@@ -953,10 +1076,13 @@
       <c t="s" r="F36">
         <v>12</v>
       </c>
+      <c t="s" r="G36">
+        <v>13</v>
+      </c>
     </row>
     <row r="37">
       <c t="s" s="3" r="A37">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c s="2" r="C37">
         <v>872</v>
@@ -968,12 +1094,15 @@
         <v>48</v>
       </c>
       <c t="s" r="F37">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G37">
+        <v>19</v>
       </c>
     </row>
     <row r="38">
       <c t="s" s="3" r="A38">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c s="2" r="C38">
         <v>1188</v>
@@ -985,12 +1114,15 @@
         <v>33</v>
       </c>
       <c t="s" r="F38">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G38">
+        <v>17</v>
       </c>
     </row>
     <row r="39">
       <c t="s" s="3" r="A39">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c s="2" r="C39">
         <v>3919</v>
@@ -1002,12 +1134,15 @@
         <v>21</v>
       </c>
       <c t="s" r="F39">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G39">
+        <v>19</v>
       </c>
     </row>
     <row r="40">
       <c t="s" s="3" r="A40">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c s="2" r="C40">
         <v>1300</v>
@@ -1019,12 +1154,15 @@
         <v>53</v>
       </c>
       <c t="s" r="F40">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G40">
+        <v>53</v>
       </c>
     </row>
     <row r="41">
       <c t="s" s="3" r="A41">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c s="2" r="C41">
         <v>1226</v>
@@ -1038,10 +1176,13 @@
       <c t="s" r="F41">
         <v>12</v>
       </c>
+      <c t="s" r="G41">
+        <v>13</v>
+      </c>
     </row>
     <row r="42">
       <c t="s" s="3" r="A42">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c s="2" r="C42">
         <v>1759</v>
@@ -1055,10 +1196,13 @@
       <c t="s" r="F42">
         <v>12</v>
       </c>
+      <c t="s" r="G42">
+        <v>13</v>
+      </c>
     </row>
     <row r="43">
       <c t="s" s="3" r="A43">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c s="2" r="C43">
         <v>11818</v>
@@ -1070,12 +1214,15 @@
         <v>52</v>
       </c>
       <c t="s" r="F43">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G43">
+        <v>13</v>
       </c>
     </row>
     <row r="44">
       <c t="s" s="3" r="A44">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c s="2" r="C44">
         <v>903</v>
@@ -1089,10 +1236,13 @@
       <c t="s" r="F44">
         <v>12</v>
       </c>
+      <c t="s" r="G44">
+        <v>13</v>
+      </c>
     </row>
     <row r="45">
       <c t="s" s="3" r="A45">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c s="2" r="C45">
         <v>600</v>
@@ -1104,12 +1254,15 @@
         <v>8</v>
       </c>
       <c t="s" r="F45">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G45">
+        <v>19</v>
       </c>
     </row>
     <row r="46">
       <c t="s" s="3" r="A46">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c s="2" r="C46">
         <v>12161</v>
@@ -1123,10 +1276,13 @@
       <c t="s" r="F46">
         <v>12</v>
       </c>
+      <c t="s" r="G46">
+        <v>13</v>
+      </c>
     </row>
     <row r="47">
       <c t="s" s="3" r="A47">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c s="2" r="C47">
         <v>1546</v>
@@ -1135,12 +1291,15 @@
         <v>8260490</v>
       </c>
       <c t="s" r="F47">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G47">
+        <v>17</v>
       </c>
     </row>
     <row r="48">
       <c t="s" s="3" r="A48">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c s="2" r="C48">
         <v>2300</v>
@@ -1152,12 +1311,15 @@
         <v>13</v>
       </c>
       <c t="s" r="F48">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G48">
+        <v>19</v>
       </c>
     </row>
     <row r="49">
       <c t="s" s="3" r="A49">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c s="2" r="C49">
         <v>5245</v>
@@ -1169,12 +1331,15 @@
         <v>37</v>
       </c>
       <c t="s" r="F49">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G49">
+        <v>13</v>
       </c>
     </row>
     <row r="50">
       <c t="s" s="3" r="A50">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c s="2" r="C50">
         <v>723</v>
@@ -1186,12 +1351,15 @@
         <v>35</v>
       </c>
       <c t="s" r="F50">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G50">
+        <v>13</v>
       </c>
     </row>
     <row r="51">
       <c t="s" s="3" r="A51">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c s="2" r="C51">
         <v>1700</v>
@@ -1203,12 +1371,15 @@
         <v>30</v>
       </c>
       <c t="s" r="F51">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G51">
+        <v>13</v>
       </c>
     </row>
     <row r="52">
       <c t="s" s="3" r="A52">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c s="2" r="C52">
         <v>8800</v>
@@ -1220,12 +1391,15 @@
         <v>41</v>
       </c>
       <c t="s" r="F52">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G52">
+        <v>13</v>
       </c>
     </row>
     <row r="53">
       <c t="s" s="3" r="A53">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c s="2" r="C53">
         <v>1700</v>
@@ -1237,12 +1411,15 @@
         <v>29</v>
       </c>
       <c t="s" r="F53">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G53">
+        <v>17</v>
       </c>
     </row>
     <row r="54">
       <c t="s" s="3" r="A54">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c s="2" r="C54">
         <v>931</v>
@@ -1254,12 +1431,15 @@
         <v>37</v>
       </c>
       <c t="s" r="F54">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c t="s" r="G54">
+        <v>13</v>
       </c>
     </row>
     <row r="55">
       <c t="s" s="3" r="A55">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c s="2" r="C55">
         <v>2607</v>
@@ -1271,7 +1451,10 @@
         <v>20</v>
       </c>
       <c t="s" r="F55">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c t="s" r="G55">
+        <v>13</v>
       </c>
     </row>
     <row r="56">
@@ -1455,14 +1638,31 @@
       <c s="2" r="C100"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1 G2 G3 G4 G5 G6 G7 G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25 G26 G27 G28 G29 G30 G31 G32 G33 G34 G35 G36 G37 G38 G39 G40 G41 G42 G43 G44 G45 G46 G47 G48 G49 G50 G51 G52 G53 G54 G55 G56 G57 G58 G59 G60 G61 G62 G63 G64 G65 G66 G67 G68 G69 G70 G71 G72 G73 G74 G75 G76 G77 G78 G79 G80 G81 G82 G83 G84 G85 G86 G87 G88 G89 G90 G91 G92 G93 G94 G95 G96 G97 G98 G99 G100">
+    <cfRule priority="1" type="cellIs" operator="equal" stopIfTrue="1" dxfId="0">
+      <formula>"Avoid all but essential travel to part(s) of country"</formula>
+    </cfRule>
+    <cfRule priority="2" type="cellIs" operator="equal" stopIfTrue="1" dxfId="1">
+      <formula>"No restrictions in this travel advice"</formula>
+    </cfRule>
+    <cfRule priority="3" type="cellIs" operator="equal" stopIfTrue="1" dxfId="2">
+      <formula>"Avoid all travel to part(s) of country"</formula>
+    </cfRule>
+    <cfRule priority="4" type="cellIs" operator="equal" stopIfTrue="1" dxfId="2">
+      <formula>"Avoid all travel to whole country"</formula>
+    </cfRule>
+    <cfRule priority="5" type="cellIs" operator="equal" stopIfTrue="1" dxfId="0">
+      <formula>"Avoid all but essential travel to whole country"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F1 F2 F3 F4 F5 F6 F7 F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25 F26 F27 F28 F29 F30 F31 F32 F33 F34 F35 F36 F37 F38 F39 F40 F41 F42 F43 F44 F45 F46 F47 F48 F49 F50 F51 F52 F53 F54 F55 F56 F57 F58 F59 F60 F61 F62 F63 F64 F65 F66 F67 F68 F69 F70 F71 F72 F73 F74 F75 F76 F77 F78 F79 F80 F81 F82 F83 F84 F85 F86 F87 F88 F89 F90 F91 F92 F93 F94 F95 F96 F97 F98 F99 F100">
-    <cfRule priority="1" type="cellIs" operator="equal" stopIfTrue="1" dxfId="0">
+    <cfRule priority="1" type="cellIs" operator="equal" stopIfTrue="1" dxfId="1">
       <formula>"Free"</formula>
     </cfRule>
-    <cfRule priority="2" type="cellIs" operator="equal" stopIfTrue="1" dxfId="1">
+    <cfRule priority="2" type="cellIs" operator="equal" stopIfTrue="1" dxfId="3">
       <formula>"Partly Free"</formula>
     </cfRule>
-    <cfRule priority="3" type="cellIs" operator="equal" stopIfTrue="1" dxfId="2">
+    <cfRule priority="3" type="cellIs" operator="equal" stopIfTrue="1" dxfId="4">
       <formula>"Not Free"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Conditional formatting and Filtering
Added Conditional formatting and filtered candidate countries by FCO
travel advice
</commit_message>
<xml_diff>
--- a/Africa.xlsx
+++ b/Africa.xlsx
@@ -94,6 +94,9 @@
     <t>Democratic Republic of the Congo</t>
   </si>
   <si>
+    <t>Democratic Republic of the congo</t>
+  </si>
+  <si>
     <t>Djibouti</t>
   </si>
   <si>
@@ -164,9 +167,6 @@
   </si>
   <si>
     <t>Nigeria</t>
-  </si>
-  <si>
-    <t>Democratic Republic of the congo</t>
   </si>
   <si>
     <t>Rwanda</t>
@@ -380,7 +380,7 @@
       <c s="3" r="S1"/>
       <c s="3" r="T1"/>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c t="s" s="3" r="A2">
         <v>7</v>
       </c>
@@ -400,7 +400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c t="s" s="3" r="A3">
         <v>10</v>
       </c>
@@ -460,7 +460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c t="s" s="3" r="A6">
         <v>15</v>
       </c>
@@ -480,7 +480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c t="s" s="3" r="A7">
         <v>18</v>
       </c>
@@ -500,7 +500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c t="s" s="3" r="A8">
         <v>20</v>
       </c>
@@ -540,7 +540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="1">
       <c t="s" s="3" r="A10">
         <v>22</v>
       </c>
@@ -560,7 +560,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c t="s" s="3" r="A11">
         <v>23</v>
       </c>
@@ -600,7 +600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c t="s" s="3" r="A13">
         <v>25</v>
       </c>
@@ -620,7 +620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c t="s" s="3" r="A14">
         <v>26</v>
       </c>
@@ -640,64 +640,64 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c t="s" s="3" r="A15">
         <v>27</v>
       </c>
       <c s="2" r="C15">
-        <v>2070</v>
+        <v>3919</v>
       </c>
       <c r="D15">
-        <v>906000</v>
+        <v>4012809</v>
       </c>
       <c r="E15">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c t="s" r="F15">
         <v>8</v>
       </c>
       <c t="s" r="G15">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" hidden="1">
       <c t="s" s="3" r="A16">
         <v>28</v>
       </c>
       <c s="2" r="C16">
-        <v>4836</v>
+        <v>2070</v>
       </c>
       <c r="D16">
-        <v>80335036</v>
+        <v>906000</v>
       </c>
       <c r="E16">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c t="s" r="F16">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c t="s" r="G16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" hidden="1">
       <c t="s" s="3" r="A17">
         <v>29</v>
       </c>
       <c s="2" r="C17">
-        <v>16312</v>
+        <v>4836</v>
       </c>
       <c r="D17">
-        <v>504000</v>
+        <v>80335036</v>
       </c>
       <c r="E17">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c t="s" r="F17">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c t="s" r="G17">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -705,33 +705,33 @@
         <v>30</v>
       </c>
       <c s="2" r="C18">
-        <v>1000</v>
+        <v>16312</v>
       </c>
       <c r="D18">
-        <v>5880000</v>
+        <v>504000</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c t="s" r="F18">
         <v>8</v>
       </c>
       <c t="s" r="G18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" hidden="1">
       <c t="s" s="3" r="A19">
         <v>31</v>
       </c>
       <c s="2" r="C19">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="D19">
-        <v>85237338</v>
+        <v>5880000</v>
       </c>
       <c r="E19">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c t="s" r="F19">
         <v>8</v>
@@ -740,24 +740,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c t="s" s="3" r="A20">
         <v>32</v>
       </c>
       <c s="2" r="C20">
-        <v>7055</v>
+        <v>1100</v>
       </c>
       <c r="D20">
-        <v>1384000</v>
+        <v>85237338</v>
       </c>
       <c r="E20">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c t="s" r="F20">
         <v>8</v>
       </c>
       <c t="s" r="G20">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
@@ -765,13 +765,13 @@
         <v>33</v>
       </c>
       <c s="2" r="C21">
-        <v>2002</v>
+        <v>7055</v>
       </c>
       <c r="D21">
-        <v>1517000</v>
+        <v>1384000</v>
       </c>
       <c r="E21">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c t="s" r="F21">
         <v>8</v>
@@ -785,16 +785,16 @@
         <v>34</v>
       </c>
       <c s="2" r="C22">
-        <v>2700</v>
+        <v>2002</v>
       </c>
       <c r="D22">
-        <v>23000000</v>
+        <v>1517000</v>
       </c>
       <c r="E22">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c t="s" r="F22">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c t="s" r="G22">
         <v>13</v>
@@ -805,16 +805,16 @@
         <v>35</v>
       </c>
       <c s="2" r="C23">
-        <v>2035</v>
+        <v>2700</v>
       </c>
       <c r="D23">
-        <v>9402000</v>
+        <v>23000000</v>
       </c>
       <c r="E23">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c t="s" r="F23">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c t="s" r="G23">
         <v>13</v>
@@ -825,16 +825,16 @@
         <v>36</v>
       </c>
       <c s="2" r="C24">
-        <v>736</v>
+        <v>2035</v>
       </c>
       <c r="D24">
-        <v>1586000</v>
+        <v>9402000</v>
       </c>
       <c r="E24">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c t="s" r="F24">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c t="s" r="G24">
         <v>13</v>
@@ -845,39 +845,39 @@
         <v>37</v>
       </c>
       <c s="2" r="C25">
-        <v>1445</v>
+        <v>736</v>
       </c>
       <c r="D25">
-        <v>34707817</v>
+        <v>1586000</v>
       </c>
       <c r="E25">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c t="s" r="F25">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c t="s" r="G25">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" hidden="1">
       <c t="s" s="3" r="A26">
         <v>38</v>
       </c>
       <c s="2" r="C26">
-        <v>2113</v>
+        <v>1445</v>
       </c>
       <c r="D26">
-        <v>1795000</v>
+        <v>34707817</v>
       </c>
       <c r="E26">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c t="s" r="F26">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c t="s" r="G26">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
@@ -885,53 +885,53 @@
         <v>39</v>
       </c>
       <c s="2" r="C27">
-        <v>1003</v>
+        <v>2113</v>
       </c>
       <c r="D27">
-        <v>3283000</v>
+        <v>1795000</v>
       </c>
       <c r="E27">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c t="s" r="F27">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c t="s" r="G27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" hidden="1">
       <c t="s" s="3" r="A28">
         <v>40</v>
       </c>
       <c s="2" r="C28">
-        <v>12700</v>
+        <v>1003</v>
       </c>
       <c r="D28">
-        <v>6036914</v>
+        <v>3283000</v>
       </c>
       <c r="E28">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c t="s" r="F28">
         <v>16</v>
       </c>
       <c t="s" r="G28">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" hidden="1">
       <c t="s" s="3" r="A29">
         <v>41</v>
       </c>
       <c s="2" r="C29">
-        <v>905</v>
+        <v>12700</v>
       </c>
       <c r="D29">
-        <v>18606000</v>
+        <v>6036914</v>
       </c>
       <c r="E29">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c t="s" r="F29">
         <v>16</v>
@@ -940,24 +940,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c t="s" s="3" r="A30">
         <v>42</v>
       </c>
       <c s="2" r="C30">
-        <v>596</v>
+        <v>905</v>
       </c>
       <c r="D30">
-        <v>12884000</v>
+        <v>18606000</v>
       </c>
       <c r="E30">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c t="s" r="F30">
         <v>16</v>
       </c>
       <c t="s" r="G30">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31">
@@ -965,33 +965,33 @@
         <v>43</v>
       </c>
       <c s="2" r="C31">
-        <v>1154</v>
+        <v>596</v>
       </c>
       <c r="D31">
-        <v>13518000</v>
+        <v>12884000</v>
       </c>
       <c r="E31">
         <v>37</v>
       </c>
       <c t="s" r="F31">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c t="s" r="G31">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" hidden="1">
       <c t="s" s="3" r="A32">
         <v>44</v>
       </c>
       <c s="2" r="C32">
-        <v>2402</v>
+        <v>1154</v>
       </c>
       <c r="D32">
-        <v>3069000</v>
+        <v>13518000</v>
       </c>
       <c r="E32">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c t="s" r="F32">
         <v>8</v>
@@ -1000,24 +1000,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c t="s" s="3" r="A33">
         <v>45</v>
       </c>
       <c s="2" r="C33">
-        <v>13703</v>
+        <v>2402</v>
       </c>
       <c r="D33">
-        <v>1219220</v>
+        <v>3069000</v>
       </c>
       <c r="E33">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c t="s" r="F33">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c t="s" r="G33">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34">
@@ -1025,16 +1025,16 @@
         <v>46</v>
       </c>
       <c s="2" r="C34">
-        <v>4600</v>
+        <v>13703</v>
       </c>
       <c r="D34">
-        <v>35757175</v>
+        <v>1219220</v>
       </c>
       <c r="E34">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c t="s" r="F34">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c t="s" r="G34">
         <v>13</v>
@@ -1045,13 +1045,13 @@
         <v>47</v>
       </c>
       <c s="2" r="C35">
-        <v>1389</v>
+        <v>4600</v>
       </c>
       <c r="D35">
-        <v>20366795</v>
+        <v>35757175</v>
       </c>
       <c r="E35">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c t="s" r="F35">
         <v>16</v>
@@ -1065,16 +1065,16 @@
         <v>48</v>
       </c>
       <c s="2" r="C36">
-        <v>7478</v>
+        <v>1389</v>
       </c>
       <c r="D36">
-        <v>2031000</v>
+        <v>20366795</v>
       </c>
       <c r="E36">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c t="s" r="F36">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c t="s" r="G36">
         <v>13</v>
@@ -1085,62 +1085,62 @@
         <v>49</v>
       </c>
       <c s="2" r="C37">
-        <v>872</v>
+        <v>7478</v>
       </c>
       <c r="D37">
-        <v>13957000</v>
+        <v>2031000</v>
       </c>
       <c r="E37">
         <v>48</v>
       </c>
       <c t="s" r="F37">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c t="s" r="G37">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" hidden="1">
       <c t="s" s="3" r="A38">
         <v>50</v>
       </c>
       <c s="2" r="C38">
-        <v>1188</v>
+        <v>872</v>
       </c>
       <c r="D38">
-        <v>154729000</v>
+        <v>13957000</v>
       </c>
       <c r="E38">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c t="s" r="F38">
         <v>16</v>
       </c>
       <c t="s" r="G38">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" hidden="1">
       <c t="s" s="3" r="A39">
         <v>51</v>
       </c>
       <c s="2" r="C39">
-        <v>3919</v>
+        <v>1188</v>
       </c>
       <c r="D39">
-        <v>4012809</v>
+        <v>154729000</v>
       </c>
       <c r="E39">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c t="s" r="F39">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c t="s" r="G39">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" hidden="1">
       <c t="s" s="3" r="A40">
         <v>52</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="1">
       <c t="s" s="3" r="A45">
         <v>58</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="1">
       <c t="s" s="3" r="A47">
         <v>60</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1">
       <c t="s" s="3" r="A48">
         <v>61</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="1">
       <c t="s" s="3" r="A53">
         <v>66</v>
       </c>
@@ -1457,187 +1457,195 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="1">
       <c s="3" r="A56"/>
       <c s="2" r="C56"/>
     </row>
-    <row r="57">
+    <row r="57" hidden="1">
       <c s="3" r="A57"/>
       <c s="2" r="C57"/>
     </row>
-    <row r="58">
+    <row r="58" hidden="1">
       <c s="3" r="A58"/>
       <c s="2" r="C58"/>
     </row>
-    <row r="59">
+    <row r="59" hidden="1">
       <c s="3" r="A59"/>
       <c s="2" r="C59"/>
     </row>
-    <row r="60">
+    <row r="60" hidden="1">
       <c s="3" r="A60"/>
       <c s="2" r="C60"/>
     </row>
-    <row r="61">
+    <row r="61" hidden="1">
       <c s="3" r="A61"/>
       <c s="2" r="C61"/>
     </row>
-    <row r="62">
+    <row r="62" hidden="1">
       <c s="3" r="A62"/>
       <c s="2" r="C62"/>
     </row>
-    <row r="63">
+    <row r="63" hidden="1">
       <c s="3" r="A63"/>
       <c s="2" r="C63"/>
     </row>
-    <row r="64">
+    <row r="64" hidden="1">
       <c s="3" r="A64"/>
       <c s="2" r="C64"/>
     </row>
-    <row r="65">
+    <row r="65" hidden="1">
       <c s="3" r="A65"/>
       <c s="2" r="C65"/>
     </row>
-    <row r="66">
+    <row r="66" hidden="1">
       <c s="3" r="A66"/>
       <c s="2" r="C66"/>
     </row>
-    <row r="67">
+    <row r="67" hidden="1">
       <c s="3" r="A67"/>
       <c s="2" r="C67"/>
     </row>
-    <row r="68">
+    <row r="68" hidden="1">
       <c s="3" r="A68"/>
       <c s="2" r="C68"/>
     </row>
-    <row r="69">
+    <row r="69" hidden="1">
       <c s="3" r="A69"/>
       <c s="2" r="C69"/>
     </row>
-    <row r="70">
+    <row r="70" hidden="1">
       <c s="3" r="A70"/>
       <c s="2" r="C70"/>
     </row>
-    <row r="71">
+    <row r="71" hidden="1">
       <c s="3" r="A71"/>
       <c s="2" r="C71"/>
     </row>
-    <row r="72">
+    <row r="72" hidden="1">
       <c s="3" r="A72"/>
       <c s="2" r="C72"/>
     </row>
-    <row r="73">
+    <row r="73" hidden="1">
       <c s="3" r="A73"/>
       <c s="2" r="C73"/>
     </row>
-    <row r="74">
+    <row r="74" hidden="1">
       <c s="3" r="A74"/>
       <c s="2" r="C74"/>
     </row>
-    <row r="75">
+    <row r="75" hidden="1">
       <c s="3" r="A75"/>
       <c s="2" r="C75"/>
     </row>
-    <row r="76">
+    <row r="76" hidden="1">
       <c s="3" r="A76"/>
       <c s="2" r="C76"/>
     </row>
-    <row r="77">
+    <row r="77" hidden="1">
       <c s="3" r="A77"/>
       <c s="2" r="C77"/>
     </row>
-    <row r="78">
+    <row r="78" hidden="1">
       <c s="3" r="A78"/>
       <c s="2" r="C78"/>
     </row>
-    <row r="79">
+    <row r="79" hidden="1">
       <c s="3" r="A79"/>
       <c s="2" r="C79"/>
     </row>
-    <row r="80">
+    <row r="80" hidden="1">
       <c s="3" r="A80"/>
       <c s="2" r="C80"/>
     </row>
-    <row r="81">
+    <row r="81" hidden="1">
       <c s="3" r="A81"/>
       <c s="2" r="C81"/>
     </row>
-    <row r="82">
+    <row r="82" hidden="1">
       <c s="3" r="A82"/>
       <c s="2" r="C82"/>
     </row>
-    <row r="83">
+    <row r="83" hidden="1">
       <c s="3" r="A83"/>
       <c s="2" r="C83"/>
     </row>
-    <row r="84">
+    <row r="84" hidden="1">
       <c s="3" r="A84"/>
       <c s="2" r="C84"/>
     </row>
-    <row r="85">
+    <row r="85" hidden="1">
       <c s="3" r="A85"/>
       <c s="2" r="C85"/>
     </row>
-    <row r="86">
+    <row r="86" hidden="1">
       <c s="3" r="A86"/>
       <c s="2" r="C86"/>
     </row>
-    <row r="87">
+    <row r="87" hidden="1">
       <c s="3" r="A87"/>
       <c s="2" r="C87"/>
     </row>
-    <row r="88">
+    <row r="88" hidden="1">
       <c s="3" r="A88"/>
       <c s="2" r="C88"/>
     </row>
-    <row r="89">
+    <row r="89" hidden="1">
       <c s="3" r="A89"/>
       <c s="2" r="C89"/>
     </row>
-    <row r="90">
+    <row r="90" hidden="1">
       <c s="3" r="A90"/>
       <c s="2" r="C90"/>
     </row>
-    <row r="91">
+    <row r="91" hidden="1">
       <c s="3" r="A91"/>
       <c s="2" r="C91"/>
     </row>
-    <row r="92">
+    <row r="92" hidden="1">
       <c s="3" r="A92"/>
       <c s="2" r="C92"/>
     </row>
-    <row r="93">
+    <row r="93" hidden="1">
       <c s="3" r="A93"/>
       <c s="2" r="C93"/>
     </row>
-    <row r="94">
+    <row r="94" hidden="1">
       <c s="3" r="A94"/>
       <c s="2" r="C94"/>
     </row>
-    <row r="95">
+    <row r="95" hidden="1">
       <c s="3" r="A95"/>
       <c s="2" r="C95"/>
     </row>
-    <row r="96">
+    <row r="96" hidden="1">
       <c s="3" r="A96"/>
       <c s="2" r="C96"/>
     </row>
-    <row r="97">
+    <row r="97" hidden="1">
       <c s="3" r="A97"/>
       <c s="2" r="C97"/>
     </row>
-    <row r="98">
+    <row r="98" hidden="1">
       <c s="3" r="A98"/>
       <c s="2" r="C98"/>
     </row>
-    <row r="99">
+    <row r="99" hidden="1">
       <c s="3" r="A99"/>
       <c s="2" r="C99"/>
     </row>
-    <row r="100">
+    <row r="100" hidden="1">
       <c s="3" r="A100"/>
       <c s="2" r="C100"/>
     </row>
   </sheetData>
+  <autoFilter ref="G1:G100">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="No restrictions in this travel advice"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="G1:G100"/>
+  </autoFilter>
   <conditionalFormatting sqref="G1 G2 G3 G4 G5 G6 G7 G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25 G26 G27 G28 G29 G30 G31 G32 G33 G34 G35 G36 G37 G38 G39 G40 G41 G42 G43 G44 G45 G46 G47 G48 G49 G50 G51 G52 G53 G54 G55 G56 G57 G58 G59 G60 G61 G62 G63 G64 G65 G66 G67 G68 G69 G70 G71 G72 G73 G74 G75 G76 G77 G78 G79 G80 G81 G82 G83 G84 G85 G86 G87 G88 G89 G90 G91 G92 G93 G94 G95 G96 G97 G98 G99 G100">
     <cfRule priority="1" type="cellIs" operator="equal" stopIfTrue="1" dxfId="0">
       <formula>"Avoid all but essential travel to part(s) of country"</formula>

</xml_diff>